<commit_message>
Statistics about MSE added to part 4
</commit_message>
<xml_diff>
--- a/Networks/Parte3/Excel/Network4.xlsx
+++ b/Networks/Parte3/Excel/Network4.xlsx
@@ -464,16 +464,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.992399742986195</v>
+        <v>6.473123644325607</v>
       </c>
       <c r="C2" t="n">
-        <v>-3.115361607584886</v>
+        <v>-4.607381193671313</v>
       </c>
       <c r="D2" t="n">
-        <v>6.509189091274481</v>
+        <v>-1.141886234607804</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.9074571694696207</v>
+        <v>3.606202155191703</v>
       </c>
     </row>
     <row r="3">
@@ -483,16 +483,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.02530588994318195</v>
+        <v>3.311868186720423</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.9781551949651406</v>
+        <v>-2.068866931281668</v>
       </c>
       <c r="D3" t="n">
-        <v>2.463610012120194</v>
+        <v>-1.253255737341218</v>
       </c>
       <c r="E3" t="n">
-        <v>3.023334633946135</v>
+        <v>1.278720260749817</v>
       </c>
     </row>
     <row r="4">
@@ -502,16 +502,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.693618807278793</v>
+        <v>-10.43802135758207</v>
       </c>
       <c r="C4" t="n">
-        <v>1.995690265495933</v>
+        <v>-3.538907799284799</v>
       </c>
       <c r="D4" t="n">
-        <v>-8.604889775144191</v>
+        <v>1.460551027431167</v>
       </c>
       <c r="E4" t="n">
-        <v>1.106936683455789</v>
+        <v>-1.925301796362968</v>
       </c>
     </row>
     <row r="5">
@@ -521,16 +521,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-2.016162561158827</v>
+        <v>0.8198212490174183</v>
       </c>
       <c r="C5" t="n">
-        <v>2.555806862681343</v>
+        <v>2.678582464998535</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9346310724968041</v>
+        <v>-0.8722260191830133</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.133463750928092</v>
+        <v>-3.03262737927183</v>
       </c>
     </row>
     <row r="6">
@@ -540,16 +540,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.526680110979042</v>
+        <v>4.549684261512178</v>
       </c>
       <c r="C6" t="n">
-        <v>2.229509010943596</v>
+        <v>4.443183458040439</v>
       </c>
       <c r="D6" t="n">
-        <v>4.379522965084463</v>
+        <v>3.215193690146705</v>
       </c>
       <c r="E6" t="n">
-        <v>-3.468790923535672</v>
+        <v>-1.609457440631691</v>
       </c>
     </row>
     <row r="7">
@@ -559,16 +559,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.286771883344559</v>
+        <v>0.6853265773749967</v>
       </c>
       <c r="C7" t="n">
-        <v>-8.545326068087178</v>
+        <v>1.118973986793525</v>
       </c>
       <c r="D7" t="n">
-        <v>1.394992104309901</v>
+        <v>0.6874921761912348</v>
       </c>
       <c r="E7" t="n">
-        <v>0.05783737800959484</v>
+        <v>7.749149725933131</v>
       </c>
     </row>
   </sheetData>
@@ -624,19 +624,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-4.390035857830386</v>
+        <v>-18.99172214959324</v>
       </c>
       <c r="C2" t="n">
-        <v>-5.985822531774705</v>
+        <v>-4.122332012459756</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.737605885524056</v>
+        <v>-0.7321956849236436</v>
       </c>
       <c r="E2" t="n">
-        <v>-9.865883052535109</v>
+        <v>-11.03407452550561</v>
       </c>
       <c r="F2" t="n">
-        <v>-4.598259568341395</v>
+        <v>1.180184025604254</v>
       </c>
     </row>
     <row r="3">
@@ -646,19 +646,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.331951722016104</v>
+        <v>1.629410162324189</v>
       </c>
       <c r="C3" t="n">
-        <v>-9.54714353361236</v>
+        <v>7.225536175766389</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.3147100914771699</v>
+        <v>-9.590779546743681</v>
       </c>
       <c r="E3" t="n">
-        <v>-3.687887333112108</v>
+        <v>8.560315622877614</v>
       </c>
       <c r="F3" t="n">
-        <v>7.473668636143406</v>
+        <v>-3.690752232856454</v>
       </c>
     </row>
     <row r="4">
@@ -668,19 +668,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-9.054268163880936</v>
+        <v>7.237419701901674</v>
       </c>
       <c r="C4" t="n">
-        <v>5.224444448816967</v>
+        <v>7.835217450405891</v>
       </c>
       <c r="D4" t="n">
-        <v>-3.86142489380658</v>
+        <v>-4.879155978740124</v>
       </c>
       <c r="E4" t="n">
-        <v>-5.718326167797028</v>
+        <v>-9.563612158599508</v>
       </c>
       <c r="F4" t="n">
-        <v>8.125615136262052</v>
+        <v>-8.200205498644948</v>
       </c>
     </row>
     <row r="5">
@@ -690,19 +690,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.630457069518193</v>
+        <v>8.944480098602378</v>
       </c>
       <c r="C5" t="n">
-        <v>6.79068419089165</v>
+        <v>-11.25671029181228</v>
       </c>
       <c r="D5" t="n">
-        <v>-9.646607528009406</v>
+        <v>-8.71683329159104</v>
       </c>
       <c r="E5" t="n">
-        <v>8.407713907826864</v>
+        <v>-2.258608497314561</v>
       </c>
       <c r="F5" t="n">
-        <v>-8.216308862190841</v>
+        <v>11.08050166900075</v>
       </c>
     </row>
     <row r="6">
@@ -712,19 +712,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-11.6578995476367</v>
+        <v>8.990569027750178</v>
       </c>
       <c r="C6" t="n">
-        <v>-6.476629873826448</v>
+        <v>-9.528284903960067</v>
       </c>
       <c r="D6" t="n">
-        <v>7.934443770723268</v>
+        <v>5.179210161542684</v>
       </c>
       <c r="E6" t="n">
-        <v>9.748175293126748</v>
+        <v>7.285550227792794</v>
       </c>
       <c r="F6" t="n">
-        <v>-8.236350070575366</v>
+        <v>-7.886814118333672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>